<commit_message>
More figures of admissions, intensive and deaths
</commit_message>
<xml_diff>
--- a/DanskeData/Admitted/Admitted.xlsx
+++ b/DanskeData/Admitted/Admitted.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>0-9</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>27_04_2021</t>
+  </si>
+  <si>
+    <t>10_11_2020</t>
   </si>
 </sst>
 </file>
@@ -450,958 +453,995 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y12"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>23</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>24</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>26</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>27</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>28</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>29</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>30</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>31</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>32</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
+        <v>39</v>
+      </c>
+      <c r="C2">
         <v>41</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>49</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>53</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>59</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>71</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>93</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>108</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>113</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>125</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>137</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>141</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>144</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>149</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>156</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>163</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>166</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>167</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>169</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>172</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>177</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>181</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>182</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>191</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
+        <v>59</v>
+      </c>
+      <c r="C3">
         <v>63</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>64</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>65</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>72</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>86</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>101</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>113</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>127</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>133</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>136</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>141</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>145</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>148</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>152</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>155</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>160</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>165</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>169</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>173</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>177</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>180</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>185</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>189</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
+        <v>172</v>
+      </c>
+      <c r="C4">
         <v>185</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>201</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>208</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>231</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>258</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>300</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>348</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>385</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>418</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>433</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>446</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>460</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>472</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>480</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>491</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>502</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>513</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>528</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>538</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>562</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>574</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>593</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>616</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>634</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
+        <v>270</v>
+      </c>
+      <c r="C5">
         <v>288</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>307</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>319</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>351</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>399</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>469</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>519</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>577</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>614</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>646</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>673</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>701</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>713</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>730</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>744</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>767</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>788</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>806</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>823</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>847</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>873</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>899</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>931</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>961</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
+        <v>427</v>
+      </c>
+      <c r="C6">
         <v>453</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>481</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>513</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>554</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>613</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>708</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>806</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>878</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>927</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>973</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>1026</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>1058</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>1077</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>1096</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>1112</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>1134</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>1167</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>1192</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>1222</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>1254</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>1301</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>1336</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>1373</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>1405</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
+        <v>704</v>
+      </c>
+      <c r="C7">
         <v>753</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>802</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>847</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>908</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>1010</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1153</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>1301</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>1422</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>1530</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>1617</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>1676</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>1706</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>1731</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>1764</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>1793</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>1831</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>1861</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>1906</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>1957</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>2010</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>2061</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>2112</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>2156</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>2202</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
+        <v>704</v>
+      </c>
+      <c r="C8">
         <v>759</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>809</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>842</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>909</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>1025</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>1177</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>1347</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>1508</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>1624</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>1721</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>1799</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>1849</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>1888</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>1916</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>1947</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>1977</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>2015</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>2043</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>2076</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>2111</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>2140</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>2170</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>2209</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>2243</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
+        <v>990</v>
+      </c>
+      <c r="C9">
         <v>1053</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>1112</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1175</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>1285</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>1405</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>1641</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>1926</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>2137</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>2343</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>2510</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>2626</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>2711</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>2770</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>2818</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>2844</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>2871</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>2909</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>2940</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>2974</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>3025</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>3064</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>3099</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>3142</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>3166</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
+        <v>746</v>
+      </c>
+      <c r="C10">
         <v>788</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>858</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>917</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>997</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>1100</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>1285</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>1497</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>1721</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>1932</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>2084</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>2225</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>2292</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>2327</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>2356</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>2393</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>2414</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>2438</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>2453</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>2472</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>2489</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>2506</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>2519</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>2531</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>2540</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
+        <v>196</v>
+      </c>
+      <c r="C11">
         <v>210</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>221</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>236</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>257</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>293</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>347</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>408</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>481</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>539</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>596</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>617</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>647</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>661</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>669</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>674</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>683</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>686</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>687</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>690</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>692</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>693</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>695</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>697</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>699</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
         <f>SUM(B2:B11)</f>
+        <v>4307</v>
+      </c>
+      <c r="C12">
+        <f>SUM(C2:C11)</f>
         <v>4593</v>
       </c>
-      <c r="C12">
-        <f t="shared" ref="C12:Y12" si="0">SUM(C2:C11)</f>
+      <c r="D12">
+        <f t="shared" ref="D12:Z12" si="0">SUM(D2:D11)</f>
         <v>4904</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <f t="shared" si="0"/>
         <v>5175</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <f t="shared" si="0"/>
         <v>5623</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <f t="shared" si="0"/>
         <v>6260</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f t="shared" si="0"/>
         <v>7274</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <f t="shared" si="0"/>
         <v>8373</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <f t="shared" si="0"/>
         <v>9349</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <f t="shared" si="0"/>
         <v>10185</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <f t="shared" si="0"/>
         <v>10853</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <f t="shared" si="0"/>
         <v>11370</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <f t="shared" si="0"/>
         <v>11713</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <f t="shared" si="0"/>
         <v>11936</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <f t="shared" si="0"/>
         <v>12137</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <f t="shared" si="0"/>
         <v>12316</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <f t="shared" si="0"/>
         <v>12505</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <f t="shared" si="0"/>
         <v>12709</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <f t="shared" si="0"/>
         <v>12893</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <f t="shared" si="0"/>
         <v>13097</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <f t="shared" si="0"/>
         <v>13344</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <f t="shared" si="0"/>
         <v>13573</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <f t="shared" si="0"/>
         <v>13790</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <f t="shared" si="0"/>
         <v>14035</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <f t="shared" si="0"/>
         <v>14240</v>
       </c>
@@ -1413,6 +1453,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010067B0F61001E26E4990655038295DAB15" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ee3cdd56ad75a133cec0310dc1ffbdf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c985db34-e54d-4323-9c17-343881a3f777" xmlns:ns4="43c47581-a1ab-43e4-9644-f9cb95e620d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dce359d01537b7c93672f0fb6f914998" ns3:_="" ns4:_="">
     <xsd:import namespace="c985db34-e54d-4323-9c17-343881a3f777"/>
@@ -1615,15 +1664,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1631,6 +1671,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B0378E4-CD70-4312-8DC0-09A17EAA3240}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1645,14 +1693,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Nursing homes, new weekly figures, age groups and more
</commit_message>
<xml_diff>
--- a/DanskeData/Admitted/Admitted.xlsx
+++ b/DanskeData/Admitted/Admitted.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>0-9</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>10_11_2020</t>
+  </si>
+  <si>
+    <t>04_05_2021</t>
   </si>
 </sst>
 </file>
@@ -453,15 +456,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:AA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -540,8 +543,11 @@
       <c r="Z1" t="s">
         <v>35</v>
       </c>
+      <c r="AA1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,8 +626,11 @@
       <c r="Z2">
         <v>196</v>
       </c>
+      <c r="AA2">
+        <v>197</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -700,8 +709,11 @@
       <c r="Z3">
         <v>194</v>
       </c>
+      <c r="AA3">
+        <v>199</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -780,8 +792,11 @@
       <c r="Z4">
         <v>634</v>
       </c>
+      <c r="AA4">
+        <v>647</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -860,8 +875,11 @@
       <c r="Z5">
         <v>961</v>
       </c>
+      <c r="AA5">
+        <v>993</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -940,8 +958,11 @@
       <c r="Z6">
         <v>1405</v>
       </c>
+      <c r="AA6">
+        <v>1440</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1020,8 +1041,11 @@
       <c r="Z7">
         <v>2202</v>
       </c>
+      <c r="AA7">
+        <v>2252</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1100,8 +1124,11 @@
       <c r="Z8">
         <v>2243</v>
       </c>
+      <c r="AA8">
+        <v>2283</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1180,8 +1207,11 @@
       <c r="Z9">
         <v>3166</v>
       </c>
+      <c r="AA9">
+        <v>3190</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1260,8 +1290,11 @@
       <c r="Z10">
         <v>2540</v>
       </c>
+      <c r="AA10">
+        <v>2547</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1340,8 +1373,11 @@
       <c r="Z11">
         <v>699</v>
       </c>
+      <c r="AA11">
+        <v>702</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1354,7 +1390,7 @@
         <v>4593</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:Z12" si="0">SUM(D2:D11)</f>
+        <f t="shared" ref="D12:AA12" si="0">SUM(D2:D11)</f>
         <v>4904</v>
       </c>
       <c r="E12">
@@ -1444,6 +1480,10 @@
       <c r="Z12">
         <f t="shared" si="0"/>
         <v>14240</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="0"/>
+        <v>14450</v>
       </c>
     </row>
   </sheetData>
@@ -1453,15 +1493,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010067B0F61001E26E4990655038295DAB15" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ee3cdd56ad75a133cec0310dc1ffbdf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c985db34-e54d-4323-9c17-343881a3f777" xmlns:ns4="43c47581-a1ab-43e4-9644-f9cb95e620d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dce359d01537b7c93672f0fb6f914998" ns3:_="" ns4:_="">
     <xsd:import namespace="c985db34-e54d-4323-9c17-343881a3f777"/>
@@ -1664,6 +1695,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1671,14 +1711,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B0378E4-CD70-4312-8DC0-09A17EAA3240}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1693,6 +1725,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added the weekly image files, and wrote into excel files
</commit_message>
<xml_diff>
--- a/DanskeData/Admitted/Admitted.xlsx
+++ b/DanskeData/Admitted/Admitted.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>0-9</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>04_05_2021</t>
+  </si>
+  <si>
+    <t>11_05_2021</t>
   </si>
 </sst>
 </file>
@@ -456,15 +459,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA12"/>
+  <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -546,8 +549,11 @@
       <c r="AA1" t="s">
         <v>37</v>
       </c>
+      <c r="AB1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,8 +635,11 @@
       <c r="AA2">
         <v>197</v>
       </c>
+      <c r="AB2">
+        <v>206</v>
+      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -712,8 +721,11 @@
       <c r="AA3">
         <v>199</v>
       </c>
+      <c r="AB3">
+        <v>209</v>
+      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -795,8 +807,11 @@
       <c r="AA4">
         <v>647</v>
       </c>
+      <c r="AB4">
+        <v>675</v>
+      </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -878,8 +893,11 @@
       <c r="AA5">
         <v>993</v>
       </c>
+      <c r="AB5">
+        <v>1034</v>
+      </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -961,8 +979,11 @@
       <c r="AA6">
         <v>1440</v>
       </c>
+      <c r="AB6">
+        <v>1483</v>
+      </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1044,8 +1065,11 @@
       <c r="AA7">
         <v>2252</v>
       </c>
+      <c r="AB7">
+        <v>2321</v>
+      </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1127,8 +1151,11 @@
       <c r="AA8">
         <v>2283</v>
       </c>
+      <c r="AB8">
+        <v>2331</v>
+      </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1210,8 +1237,11 @@
       <c r="AA9">
         <v>3190</v>
       </c>
+      <c r="AB9">
+        <v>3207</v>
+      </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1293,8 +1323,11 @@
       <c r="AA10">
         <v>2547</v>
       </c>
+      <c r="AB10">
+        <v>2559</v>
+      </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1376,8 +1409,11 @@
       <c r="AA11">
         <v>702</v>
       </c>
+      <c r="AB11">
+        <v>704</v>
+      </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1390,7 +1426,7 @@
         <v>4593</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:AA12" si="0">SUM(D2:D11)</f>
+        <f t="shared" ref="D12:AB12" si="0">SUM(D2:D11)</f>
         <v>4904</v>
       </c>
       <c r="E12">
@@ -1484,6 +1520,10 @@
       <c r="AA12">
         <f t="shared" si="0"/>
         <v>14450</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="0"/>
+        <v>14729</v>
       </c>
     </row>
   </sheetData>
@@ -1493,6 +1533,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010067B0F61001E26E4990655038295DAB15" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ee3cdd56ad75a133cec0310dc1ffbdf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c985db34-e54d-4323-9c17-343881a3f777" xmlns:ns4="43c47581-a1ab-43e4-9644-f9cb95e620d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dce359d01537b7c93672f0fb6f914998" ns3:_="" ns4:_="">
     <xsd:import namespace="c985db34-e54d-4323-9c17-343881a3f777"/>
@@ -1695,15 +1744,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1711,6 +1751,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B0378E4-CD70-4312-8DC0-09A17EAA3240}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1725,14 +1773,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added weekly data to excel files
</commit_message>
<xml_diff>
--- a/DanskeData/Admitted/Admitted.xlsx
+++ b/DanskeData/Admitted/Admitted.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>0-9</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>11_05_2021</t>
+  </si>
+  <si>
+    <t>18_05_2021</t>
   </si>
 </sst>
 </file>
@@ -459,15 +462,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB12"/>
+  <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AB14" sqref="AB14"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -552,8 +555,11 @@
       <c r="AB1" t="s">
         <v>38</v>
       </c>
+      <c r="AC1" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -638,8 +644,11 @@
       <c r="AB2">
         <v>206</v>
       </c>
+      <c r="AC2">
+        <v>205</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -724,8 +733,11 @@
       <c r="AB3">
         <v>209</v>
       </c>
+      <c r="AC3">
+        <v>209</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -810,8 +822,11 @@
       <c r="AB4">
         <v>675</v>
       </c>
+      <c r="AC4">
+        <v>692</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -896,8 +911,11 @@
       <c r="AB5">
         <v>1034</v>
       </c>
+      <c r="AC5">
+        <v>1050</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -982,8 +1000,11 @@
       <c r="AB6">
         <v>1483</v>
       </c>
+      <c r="AC6">
+        <v>1512</v>
+      </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1068,8 +1089,11 @@
       <c r="AB7">
         <v>2321</v>
       </c>
+      <c r="AC7">
+        <v>2369</v>
+      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1154,8 +1178,11 @@
       <c r="AB8">
         <v>2331</v>
       </c>
+      <c r="AC8">
+        <v>2365</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1240,8 +1267,11 @@
       <c r="AB9">
         <v>3207</v>
       </c>
+      <c r="AC9">
+        <v>3228</v>
+      </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1326,8 +1356,11 @@
       <c r="AB10">
         <v>2559</v>
       </c>
+      <c r="AC10">
+        <v>2561</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1412,8 +1445,11 @@
       <c r="AB11">
         <v>704</v>
       </c>
+      <c r="AC11">
+        <v>703</v>
+      </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1426,7 +1462,7 @@
         <v>4593</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:AB12" si="0">SUM(D2:D11)</f>
+        <f t="shared" ref="D12:AC12" si="0">SUM(D2:D11)</f>
         <v>4904</v>
       </c>
       <c r="E12">
@@ -1524,6 +1560,10 @@
       <c r="AB12">
         <f t="shared" si="0"/>
         <v>14729</v>
+      </c>
+      <c r="AC12">
+        <f t="shared" si="0"/>
+        <v>14894</v>
       </c>
     </row>
   </sheetData>
@@ -1533,15 +1573,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010067B0F61001E26E4990655038295DAB15" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ee3cdd56ad75a133cec0310dc1ffbdf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c985db34-e54d-4323-9c17-343881a3f777" xmlns:ns4="43c47581-a1ab-43e4-9644-f9cb95e620d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dce359d01537b7c93672f0fb6f914998" ns3:_="" ns4:_="">
     <xsd:import namespace="c985db34-e54d-4323-9c17-343881a3f777"/>
@@ -1744,6 +1775,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1751,14 +1791,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B0378E4-CD70-4312-8DC0-09A17EAA3240}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1773,6 +1805,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated the weekly data in excel files
</commit_message>
<xml_diff>
--- a/DanskeData/Admitted/Admitted.xlsx
+++ b/DanskeData/Admitted/Admitted.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>0-9</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>18_05_2021</t>
+  </si>
+  <si>
+    <t>25_05_2021</t>
   </si>
 </sst>
 </file>
@@ -462,15 +465,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC12"/>
+  <dimension ref="A1:AD12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AC14" sqref="AC14"/>
+      <selection activeCell="AC12" sqref="AC12:AD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -558,8 +561,11 @@
       <c r="AC1" t="s">
         <v>39</v>
       </c>
+      <c r="AD1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,8 +653,11 @@
       <c r="AC2">
         <v>205</v>
       </c>
+      <c r="AD2">
+        <v>216</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -736,8 +745,11 @@
       <c r="AC3">
         <v>209</v>
       </c>
+      <c r="AD3">
+        <v>213</v>
+      </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -825,8 +837,11 @@
       <c r="AC4">
         <v>692</v>
       </c>
+      <c r="AD4">
+        <v>716</v>
+      </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -914,8 +929,11 @@
       <c r="AC5">
         <v>1050</v>
       </c>
+      <c r="AD5">
+        <v>1077</v>
+      </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1003,8 +1021,11 @@
       <c r="AC6">
         <v>1512</v>
       </c>
+      <c r="AD6">
+        <v>1563</v>
+      </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1092,8 +1113,11 @@
       <c r="AC7">
         <v>2369</v>
       </c>
+      <c r="AD7">
+        <v>2415</v>
+      </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1181,8 +1205,11 @@
       <c r="AC8">
         <v>2365</v>
       </c>
+      <c r="AD8">
+        <v>2387</v>
+      </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1270,8 +1297,11 @@
       <c r="AC9">
         <v>3228</v>
       </c>
+      <c r="AD9">
+        <v>3240</v>
+      </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1359,8 +1389,11 @@
       <c r="AC10">
         <v>2561</v>
       </c>
+      <c r="AD10">
+        <v>2561</v>
+      </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1448,8 +1481,11 @@
       <c r="AC11">
         <v>703</v>
       </c>
+      <c r="AD11">
+        <v>703</v>
+      </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1462,7 +1498,7 @@
         <v>4593</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:AC12" si="0">SUM(D2:D11)</f>
+        <f t="shared" ref="D12:AD12" si="0">SUM(D2:D11)</f>
         <v>4904</v>
       </c>
       <c r="E12">
@@ -1564,6 +1600,10 @@
       <c r="AC12">
         <f t="shared" si="0"/>
         <v>14894</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="0"/>
+        <v>15091</v>
       </c>
     </row>
   </sheetData>
@@ -1573,6 +1613,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010067B0F61001E26E4990655038295DAB15" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ee3cdd56ad75a133cec0310dc1ffbdf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c985db34-e54d-4323-9c17-343881a3f777" xmlns:ns4="43c47581-a1ab-43e4-9644-f9cb95e620d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dce359d01537b7c93672f0fb6f914998" ns3:_="" ns4:_="">
     <xsd:import namespace="c985db34-e54d-4323-9c17-343881a3f777"/>
@@ -1775,15 +1824,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1791,6 +1831,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B0378E4-CD70-4312-8DC0-09A17EAA3240}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1805,14 +1853,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated with new weekly data
</commit_message>
<xml_diff>
--- a/DanskeData/Admitted/Admitted.xlsx
+++ b/DanskeData/Admitted/Admitted.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>0-9</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>15_06_2021</t>
+  </si>
+  <si>
+    <t>22_06_2021</t>
   </si>
 </sst>
 </file>
@@ -474,15 +477,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG12"/>
+  <dimension ref="A1:AH12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AG15" sqref="AG15"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AG14" sqref="AG14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -582,8 +585,11 @@
       <c r="AG1" t="s">
         <v>43</v>
       </c>
+      <c r="AH1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -683,8 +689,11 @@
       <c r="AG2">
         <v>229</v>
       </c>
+      <c r="AH2">
+        <v>231</v>
+      </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -784,8 +793,11 @@
       <c r="AG3">
         <v>233</v>
       </c>
+      <c r="AH3">
+        <v>236</v>
+      </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -885,8 +897,11 @@
       <c r="AG4">
         <v>768</v>
       </c>
+      <c r="AH4">
+        <v>772</v>
+      </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -986,8 +1001,11 @@
       <c r="AG5">
         <v>1152</v>
       </c>
+      <c r="AH5">
+        <v>1166</v>
+      </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1087,8 +1105,11 @@
       <c r="AG6">
         <v>1677</v>
       </c>
+      <c r="AH6">
+        <v>1698</v>
+      </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1188,8 +1209,11 @@
       <c r="AG7">
         <v>2534</v>
       </c>
+      <c r="AH7">
+        <v>2542</v>
+      </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1289,8 +1313,11 @@
       <c r="AG8">
         <v>2432</v>
       </c>
+      <c r="AH8">
+        <v>2437</v>
+      </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1390,8 +1417,11 @@
       <c r="AG9">
         <v>3263</v>
       </c>
+      <c r="AH9">
+        <v>3265</v>
+      </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1491,8 +1521,11 @@
       <c r="AG10">
         <v>2572</v>
       </c>
+      <c r="AH10">
+        <v>2577</v>
+      </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1592,8 +1625,11 @@
       <c r="AG11">
         <v>707</v>
       </c>
+      <c r="AH11">
+        <v>708</v>
+      </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1606,7 +1642,7 @@
         <v>4593</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:AG12" si="0">SUM(D2:D11)</f>
+        <f t="shared" ref="D12:AH12" si="0">SUM(D2:D11)</f>
         <v>4904</v>
       </c>
       <c r="E12">
@@ -1724,6 +1760,10 @@
       <c r="AG12">
         <f t="shared" si="0"/>
         <v>15567</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="0"/>
+        <v>15632</v>
       </c>
     </row>
   </sheetData>
@@ -1733,6 +1773,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010067B0F61001E26E4990655038295DAB15" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ee3cdd56ad75a133cec0310dc1ffbdf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c985db34-e54d-4323-9c17-343881a3f777" xmlns:ns4="43c47581-a1ab-43e4-9644-f9cb95e620d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dce359d01537b7c93672f0fb6f914998" ns3:_="" ns4:_="">
     <xsd:import namespace="c985db34-e54d-4323-9c17-343881a3f777"/>
@@ -1935,15 +1984,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1951,6 +1991,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B0378E4-CD70-4312-8DC0-09A17EAA3240}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1965,14 +2013,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated weekly excel files
</commit_message>
<xml_diff>
--- a/DanskeData/Admitted/Admitted.xlsx
+++ b/DanskeData/Admitted/Admitted.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>0-9</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>22_06_2021</t>
+  </si>
+  <si>
+    <t>29_06_2021</t>
   </si>
 </sst>
 </file>
@@ -477,15 +480,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AI12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AG14" sqref="AG14"/>
+      <selection activeCell="AL17" sqref="AL17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -588,8 +591,11 @@
       <c r="AH1" t="s">
         <v>44</v>
       </c>
+      <c r="AI1" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,8 +698,11 @@
       <c r="AH2">
         <v>231</v>
       </c>
+      <c r="AI2">
+        <v>233</v>
+      </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -796,8 +805,11 @@
       <c r="AH3">
         <v>236</v>
       </c>
+      <c r="AI3">
+        <v>237</v>
+      </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -900,8 +912,11 @@
       <c r="AH4">
         <v>772</v>
       </c>
+      <c r="AI4">
+        <v>779</v>
+      </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1004,8 +1019,11 @@
       <c r="AH5">
         <v>1166</v>
       </c>
+      <c r="AI5">
+        <v>1179</v>
+      </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1108,8 +1126,11 @@
       <c r="AH6">
         <v>1698</v>
       </c>
+      <c r="AI6">
+        <v>1707</v>
+      </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1212,8 +1233,11 @@
       <c r="AH7">
         <v>2542</v>
       </c>
+      <c r="AI7">
+        <v>2547</v>
+      </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1316,8 +1340,11 @@
       <c r="AH8">
         <v>2437</v>
       </c>
+      <c r="AI8">
+        <v>2444</v>
+      </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1420,8 +1447,11 @@
       <c r="AH9">
         <v>3265</v>
       </c>
+      <c r="AI9">
+        <v>3268</v>
+      </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1524,8 +1554,11 @@
       <c r="AH10">
         <v>2577</v>
       </c>
+      <c r="AI10">
+        <v>2577</v>
+      </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1628,8 +1661,11 @@
       <c r="AH11">
         <v>708</v>
       </c>
+      <c r="AI11">
+        <v>709</v>
+      </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1642,7 +1678,7 @@
         <v>4593</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:AH12" si="0">SUM(D2:D11)</f>
+        <f t="shared" ref="D12:AI12" si="0">SUM(D2:D11)</f>
         <v>4904</v>
       </c>
       <c r="E12">
@@ -1764,6 +1800,10 @@
       <c r="AH12">
         <f t="shared" si="0"/>
         <v>15632</v>
+      </c>
+      <c r="AI12">
+        <f t="shared" si="0"/>
+        <v>15680</v>
       </c>
     </row>
   </sheetData>
@@ -1773,15 +1813,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010067B0F61001E26E4990655038295DAB15" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ee3cdd56ad75a133cec0310dc1ffbdf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c985db34-e54d-4323-9c17-343881a3f777" xmlns:ns4="43c47581-a1ab-43e4-9644-f9cb95e620d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dce359d01537b7c93672f0fb6f914998" ns3:_="" ns4:_="">
     <xsd:import namespace="c985db34-e54d-4323-9c17-343881a3f777"/>
@@ -1984,6 +2015,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1991,14 +2031,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B0378E4-CD70-4312-8DC0-09A17EAA3240}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2013,6 +2045,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>